<commit_message>
Updated example to have a scale column
</commit_message>
<xml_diff>
--- a/Demos/Multi-Modal/ExamplePositionFile.xlsx
+++ b/Demos/Multi-Modal/ExamplePositionFile.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dontm\Dropbox (Personal)\Research\Projects\AdaptiveOpticsAnalysis\AutoAOMontagingGUI\Demos\AOIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dontm\Dropbox (Personal)\Research\Projects\AOAutomontaging\AOAutomontaging\Demos\Multi-Modal\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781F9D7B-8BB6-4073-82FF-622257881E2A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13" yWindow="5700" windowWidth="14173" windowHeight="5760"/>
+    <workbookView xWindow="-15" yWindow="5700" windowWidth="14175" windowHeight="5760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="151">
   <si>
     <t>0012</t>
   </si>
@@ -484,7 +485,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -630,6 +631,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -665,6 +683,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -840,26 +875,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.703125" customWidth="1"/>
-    <col min="2" max="2" width="31.1171875" customWidth="1"/>
-    <col min="3" max="3" width="18.29296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.73046875" customWidth="1"/>
+    <col min="2" max="2" width="31.1328125" customWidth="1"/>
+    <col min="3" max="3" width="18.265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -867,7 +902,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -875,22 +910,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -900,8 +935,11 @@
       <c r="C9" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -911,9 +949,12 @@
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -923,9 +964,12 @@
       <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -935,9 +979,12 @@
       <c r="C12" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -947,9 +994,12 @@
       <c r="C13" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -959,9 +1009,12 @@
       <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -971,9 +1024,12 @@
       <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -983,9 +1039,12 @@
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -995,9 +1054,12 @@
       <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1007,9 +1069,12 @@
       <c r="C18" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -1019,9 +1084,12 @@
       <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -1031,8 +1099,11 @@
       <c r="C20" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -1042,8 +1113,11 @@
       <c r="C21" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1053,8 +1127,11 @@
       <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1064,8 +1141,11 @@
       <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1075,8 +1155,11 @@
       <c r="C24" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1086,8 +1169,11 @@
       <c r="C25" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -1097,8 +1183,11 @@
       <c r="C26" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -1108,8 +1197,11 @@
       <c r="C27" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -1119,8 +1211,11 @@
       <c r="C28" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
@@ -1130,8 +1225,11 @@
       <c r="C29" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -1141,8 +1239,11 @@
       <c r="C30" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -1152,8 +1253,11 @@
       <c r="C31" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
@@ -1163,8 +1267,11 @@
       <c r="C32" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
@@ -1174,8 +1281,11 @@
       <c r="C33" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>59</v>
       </c>
@@ -1185,8 +1295,11 @@
       <c r="C34" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -1196,8 +1309,11 @@
       <c r="C35" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>13</v>
       </c>
@@ -1207,8 +1323,11 @@
       <c r="C36" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
@@ -1218,8 +1337,11 @@
       <c r="C37" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>60</v>
       </c>
@@ -1229,8 +1351,11 @@
       <c r="C38" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>61</v>
       </c>
@@ -1240,8 +1365,11 @@
       <c r="C39" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
@@ -1251,8 +1379,11 @@
       <c r="C40" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1262,8 +1393,11 @@
       <c r="C41" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
@@ -1273,8 +1407,11 @@
       <c r="C42" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>15</v>
       </c>
@@ -1284,8 +1421,11 @@
       <c r="C43" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>62</v>
       </c>
@@ -1295,8 +1435,11 @@
       <c r="C44" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>16</v>
       </c>
@@ -1306,8 +1449,11 @@
       <c r="C45" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
@@ -1317,8 +1463,11 @@
       <c r="C46" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>18</v>
       </c>
@@ -1328,8 +1477,11 @@
       <c r="C47" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -1339,8 +1491,11 @@
       <c r="C48" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
@@ -1350,8 +1505,11 @@
       <c r="C49" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>19</v>
       </c>
@@ -1361,8 +1519,11 @@
       <c r="C50" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>20</v>
       </c>
@@ -1372,8 +1533,11 @@
       <c r="C51" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>21</v>
       </c>
@@ -1383,8 +1547,11 @@
       <c r="C52" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>22</v>
       </c>
@@ -1394,8 +1561,11 @@
       <c r="C53" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>23</v>
       </c>
@@ -1405,8 +1575,11 @@
       <c r="C54" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>24</v>
       </c>
@@ -1416,8 +1589,11 @@
       <c r="C55" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>139</v>
       </c>
@@ -1427,8 +1603,11 @@
       <c r="C56" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>140</v>
       </c>
@@ -1438,8 +1617,11 @@
       <c r="C57" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>141</v>
       </c>
@@ -1449,8 +1631,11 @@
       <c r="C58" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>143</v>
       </c>
@@ -1460,8 +1645,11 @@
       <c r="C59" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>144</v>
       </c>
@@ -1471,8 +1659,11 @@
       <c r="C60" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>145</v>
       </c>
@@ -1482,8 +1673,11 @@
       <c r="C61" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>146</v>
       </c>
@@ -1493,8 +1687,11 @@
       <c r="C62" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>147</v>
       </c>
@@ -1504,8 +1701,11 @@
       <c r="C63" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>148</v>
       </c>
@@ -1514,6 +1714,9 @@
       </c>
       <c r="C64" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1528,12 +1731,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1545,12 +1748,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Revert "Updated example to have a scale column"
This reverts commit f27f23468db1847cbf8db75671a9b8549fa40b5c.
</commit_message>
<xml_diff>
--- a/Demos/Multi-Modal/ExamplePositionFile.xlsx
+++ b/Demos/Multi-Modal/ExamplePositionFile.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dontm\Dropbox (Personal)\Research\Projects\AOAutomontaging\AOAutomontaging\Demos\Multi-Modal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dontm\Dropbox (Personal)\Research\Projects\AdaptiveOpticsAnalysis\AutoAOMontagingGUI\Demos\AOIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781F9D7B-8BB6-4073-82FF-622257881E2A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5700" windowWidth="14175" windowHeight="5760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13" yWindow="5700" windowWidth="14173" windowHeight="5760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="151">
   <si>
     <t>0012</t>
   </si>
@@ -485,7 +484,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -631,23 +630,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -683,23 +665,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -875,26 +840,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D64"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="17.73046875" customWidth="1"/>
-    <col min="2" max="2" width="31.1328125" customWidth="1"/>
-    <col min="3" max="3" width="18.265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.703125" customWidth="1"/>
+    <col min="2" max="2" width="31.1171875" customWidth="1"/>
+    <col min="3" max="3" width="18.29296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -902,7 +867,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -910,22 +875,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -935,11 +900,8 @@
       <c r="C9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -949,12 +911,9 @@
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -964,12 +923,9 @@
       <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -979,12 +935,9 @@
       <c r="C12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -994,12 +947,9 @@
       <c r="C13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1009,12 +959,9 @@
       <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1024,12 +971,9 @@
       <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1039,12 +983,9 @@
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1054,12 +995,9 @@
       <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1069,12 +1007,9 @@
       <c r="C18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -1084,12 +1019,9 @@
       <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -1099,11 +1031,8 @@
       <c r="C20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -1113,11 +1042,8 @@
       <c r="C21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1127,11 +1053,8 @@
       <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1141,11 +1064,8 @@
       <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1155,11 +1075,8 @@
       <c r="C24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1169,11 +1086,8 @@
       <c r="C25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -1183,11 +1097,8 @@
       <c r="C26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -1197,11 +1108,8 @@
       <c r="C27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -1211,11 +1119,8 @@
       <c r="C28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
@@ -1225,11 +1130,8 @@
       <c r="C29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -1239,11 +1141,8 @@
       <c r="C30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -1253,11 +1152,8 @@
       <c r="C31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
@@ -1267,11 +1163,8 @@
       <c r="C32" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
@@ -1281,11 +1174,8 @@
       <c r="C33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
         <v>59</v>
       </c>
@@ -1295,11 +1185,8 @@
       <c r="C34" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -1309,11 +1196,8 @@
       <c r="C35" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
         <v>13</v>
       </c>
@@ -1323,11 +1207,8 @@
       <c r="C36" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
@@ -1337,11 +1218,8 @@
       <c r="C37" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
         <v>60</v>
       </c>
@@ -1351,11 +1229,8 @@
       <c r="C38" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
         <v>61</v>
       </c>
@@ -1365,11 +1240,8 @@
       <c r="C39" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
@@ -1379,11 +1251,8 @@
       <c r="C40" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1393,11 +1262,8 @@
       <c r="C41" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
@@ -1407,11 +1273,8 @@
       <c r="C42" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
         <v>15</v>
       </c>
@@ -1421,11 +1284,8 @@
       <c r="C43" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
         <v>62</v>
       </c>
@@ -1435,11 +1295,8 @@
       <c r="C44" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
         <v>16</v>
       </c>
@@ -1449,11 +1306,8 @@
       <c r="C45" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
@@ -1463,11 +1317,8 @@
       <c r="C46" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
         <v>18</v>
       </c>
@@ -1477,11 +1328,8 @@
       <c r="C47" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -1491,11 +1339,8 @@
       <c r="C48" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
@@ -1505,11 +1350,8 @@
       <c r="C49" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A50" s="1" t="s">
         <v>19</v>
       </c>
@@ -1519,11 +1361,8 @@
       <c r="C50" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51" s="1" t="s">
         <v>20</v>
       </c>
@@ -1533,11 +1372,8 @@
       <c r="C51" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A52" s="1" t="s">
         <v>21</v>
       </c>
@@ -1547,11 +1383,8 @@
       <c r="C52" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A53" s="1" t="s">
         <v>22</v>
       </c>
@@ -1561,11 +1394,8 @@
       <c r="C53" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A54" s="1" t="s">
         <v>23</v>
       </c>
@@ -1575,11 +1405,8 @@
       <c r="C54" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A55" s="1" t="s">
         <v>24</v>
       </c>
@@ -1589,11 +1416,8 @@
       <c r="C55" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
         <v>139</v>
       </c>
@@ -1603,11 +1427,8 @@
       <c r="C56" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
         <v>140</v>
       </c>
@@ -1617,11 +1438,8 @@
       <c r="C57" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A58" s="1" t="s">
         <v>141</v>
       </c>
@@ -1631,11 +1449,8 @@
       <c r="C58" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A59" s="1" t="s">
         <v>143</v>
       </c>
@@ -1645,11 +1460,8 @@
       <c r="C59" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A60" s="1" t="s">
         <v>144</v>
       </c>
@@ -1659,11 +1471,8 @@
       <c r="C60" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A61" s="1" t="s">
         <v>145</v>
       </c>
@@ -1673,11 +1482,8 @@
       <c r="C61" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A62" s="1" t="s">
         <v>146</v>
       </c>
@@ -1687,11 +1493,8 @@
       <c r="C62" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A63" s="1" t="s">
         <v>147</v>
       </c>
@@ -1701,11 +1504,8 @@
       <c r="C63" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A64" s="1" t="s">
         <v>148</v>
       </c>
@@ -1714,9 +1514,6 @@
       </c>
       <c r="C64" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1731,12 +1528,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1748,12 +1545,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Revert "Revert "Updated example to have a scale column""
This reverts commit eecb0140fcd0796904e35fe4022481563a969346.
</commit_message>
<xml_diff>
--- a/Demos/Multi-Modal/ExamplePositionFile.xlsx
+++ b/Demos/Multi-Modal/ExamplePositionFile.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dontm\Dropbox (Personal)\Research\Projects\AdaptiveOpticsAnalysis\AutoAOMontagingGUI\Demos\AOIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dontm\Dropbox (Personal)\Research\Projects\AOAutomontaging\AOAutomontaging\Demos\Multi-Modal\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781F9D7B-8BB6-4073-82FF-622257881E2A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13" yWindow="5700" windowWidth="14173" windowHeight="5760"/>
+    <workbookView xWindow="-15" yWindow="5700" windowWidth="14175" windowHeight="5760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="151">
   <si>
     <t>0012</t>
   </si>
@@ -484,7 +485,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -630,6 +631,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -665,6 +683,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -840,26 +875,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.703125" customWidth="1"/>
-    <col min="2" max="2" width="31.1171875" customWidth="1"/>
-    <col min="3" max="3" width="18.29296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.73046875" customWidth="1"/>
+    <col min="2" max="2" width="31.1328125" customWidth="1"/>
+    <col min="3" max="3" width="18.265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -867,7 +902,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -875,22 +910,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -900,8 +935,11 @@
       <c r="C9" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -911,9 +949,12 @@
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -923,9 +964,12 @@
       <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -935,9 +979,12 @@
       <c r="C12" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -947,9 +994,12 @@
       <c r="C13" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -959,9 +1009,12 @@
       <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -971,9 +1024,12 @@
       <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -983,9 +1039,12 @@
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -995,9 +1054,12 @@
       <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1007,9 +1069,12 @@
       <c r="C18" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -1019,9 +1084,12 @@
       <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -1031,8 +1099,11 @@
       <c r="C20" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -1042,8 +1113,11 @@
       <c r="C21" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1053,8 +1127,11 @@
       <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1064,8 +1141,11 @@
       <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1075,8 +1155,11 @@
       <c r="C24" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1086,8 +1169,11 @@
       <c r="C25" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -1097,8 +1183,11 @@
       <c r="C26" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -1108,8 +1197,11 @@
       <c r="C27" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -1119,8 +1211,11 @@
       <c r="C28" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
@@ -1130,8 +1225,11 @@
       <c r="C29" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -1141,8 +1239,11 @@
       <c r="C30" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -1152,8 +1253,11 @@
       <c r="C31" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
@@ -1163,8 +1267,11 @@
       <c r="C32" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
@@ -1174,8 +1281,11 @@
       <c r="C33" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>59</v>
       </c>
@@ -1185,8 +1295,11 @@
       <c r="C34" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -1196,8 +1309,11 @@
       <c r="C35" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>13</v>
       </c>
@@ -1207,8 +1323,11 @@
       <c r="C36" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
@@ -1218,8 +1337,11 @@
       <c r="C37" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>60</v>
       </c>
@@ -1229,8 +1351,11 @@
       <c r="C38" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>61</v>
       </c>
@@ -1240,8 +1365,11 @@
       <c r="C39" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
@@ -1251,8 +1379,11 @@
       <c r="C40" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1262,8 +1393,11 @@
       <c r="C41" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
@@ -1273,8 +1407,11 @@
       <c r="C42" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>15</v>
       </c>
@@ -1284,8 +1421,11 @@
       <c r="C43" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>62</v>
       </c>
@@ -1295,8 +1435,11 @@
       <c r="C44" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>16</v>
       </c>
@@ -1306,8 +1449,11 @@
       <c r="C45" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
@@ -1317,8 +1463,11 @@
       <c r="C46" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>18</v>
       </c>
@@ -1328,8 +1477,11 @@
       <c r="C47" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -1339,8 +1491,11 @@
       <c r="C48" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
@@ -1350,8 +1505,11 @@
       <c r="C49" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>19</v>
       </c>
@@ -1361,8 +1519,11 @@
       <c r="C50" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>20</v>
       </c>
@@ -1372,8 +1533,11 @@
       <c r="C51" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>21</v>
       </c>
@@ -1383,8 +1547,11 @@
       <c r="C52" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>22</v>
       </c>
@@ -1394,8 +1561,11 @@
       <c r="C53" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>23</v>
       </c>
@@ -1405,8 +1575,11 @@
       <c r="C54" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>24</v>
       </c>
@@ -1416,8 +1589,11 @@
       <c r="C55" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>139</v>
       </c>
@@ -1427,8 +1603,11 @@
       <c r="C56" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>140</v>
       </c>
@@ -1438,8 +1617,11 @@
       <c r="C57" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>141</v>
       </c>
@@ -1449,8 +1631,11 @@
       <c r="C58" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>143</v>
       </c>
@@ -1460,8 +1645,11 @@
       <c r="C59" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>144</v>
       </c>
@@ -1471,8 +1659,11 @@
       <c r="C60" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>145</v>
       </c>
@@ -1482,8 +1673,11 @@
       <c r="C61" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>146</v>
       </c>
@@ -1493,8 +1687,11 @@
       <c r="C62" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>147</v>
       </c>
@@ -1504,8 +1701,11 @@
       <c r="C63" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>148</v>
       </c>
@@ -1514,6 +1714,9 @@
       </c>
       <c r="C64" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1528,12 +1731,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1545,12 +1748,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>